<commit_message>
Sync: Full project structure and recent UI/Function updates for MacBook transition
</commit_message>
<xml_diff>
--- a/TÜM SÜRELER TABLOSU.xlsx
+++ b/TÜM SÜRELER TABLOSU.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\LISANS_BIRIMI\00_Lisans Süreç Takip\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4BE6EFD-8E2C-46A2-A821-91247C04774A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B833C3FA-BBFF-43BC-B458-258F42DD18E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,8 +18,8 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">ESKİ!$A$1:$A$126</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">GÜNCEL!$A$1:$A$174</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">GÜNCEL!$A$71:$E$173</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">GÜNCEL!$A$1:$A$183</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">GÜNCEL!$A$71:$E$182</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="834" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="863" uniqueCount="255">
   <si>
     <t>PROJE ADI</t>
   </si>
@@ -799,6 +799,24 @@
   </si>
   <si>
     <t>30 TAKVİM GÜNÜ</t>
+  </si>
+  <si>
+    <t>R25-BALIKESİR-2 RES</t>
+  </si>
+  <si>
+    <t>BAKANLIK İŞ PROGRAMI</t>
+  </si>
+  <si>
+    <t>+5 gün ile birlikte tebliğ tarihi 27.01.2026 olarak dikkate alırsak 30 gün sonrası 26.02.2026, 60 gün sonrası 30.03.2026.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALAPINAR RES </t>
+  </si>
+  <si>
+    <t>ÖNLİSANS İPTALİ</t>
+  </si>
+  <si>
+    <t>30.01.2026 da itiraz edildi.</t>
   </si>
 </sst>
 </file>
@@ -1451,28 +1469,26 @@
     <xf numFmtId="14" fontId="0" fillId="10" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="9" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1764,10 +1780,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:DR178"/>
+  <dimension ref="A1:DR187"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A128" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B135" sqref="B135"/>
+    <sheetView tabSelected="1" topLeftCell="A133" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C133" sqref="C133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3691,60 +3707,62 @@
       <c r="E129" s="72"/>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A130" s="142" t="s">
+      <c r="A130" s="137" t="s">
         <v>11</v>
       </c>
-      <c r="B130" s="143" t="s">
+      <c r="B130" s="138" t="s">
         <v>234</v>
       </c>
-      <c r="C130" s="143" t="s">
+      <c r="C130" s="138" t="s">
         <v>235</v>
       </c>
-      <c r="D130" s="144">
+      <c r="D130" s="139">
         <v>46038</v>
       </c>
       <c r="E130" s="72"/>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A131" s="60" t="s">
+      <c r="A131" s="62" t="s">
         <v>57</v>
       </c>
-      <c r="B131" s="2" t="s">
+      <c r="B131" s="50" t="s">
         <v>245</v>
       </c>
-      <c r="C131" s="2" t="s">
+      <c r="C131" s="50" t="s">
         <v>155</v>
       </c>
-      <c r="D131" s="66">
+      <c r="D131" s="67">
+        <v>46048</v>
+      </c>
+      <c r="E131" s="72" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A132" s="137" t="s">
+        <v>11</v>
+      </c>
+      <c r="B132" s="138" t="s">
+        <v>236</v>
+      </c>
+      <c r="C132" s="138"/>
+      <c r="D132" s="139">
+        <v>45680</v>
+      </c>
+      <c r="E132" s="133" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A133" s="142" t="s">
+        <v>238</v>
+      </c>
+      <c r="B133" s="143"/>
+      <c r="C133" s="143"/>
+      <c r="D133" s="144">
         <v>46045</v>
       </c>
-      <c r="E131" s="72"/>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A132" s="133" t="s">
-        <v>11</v>
-      </c>
-      <c r="B132" s="134" t="s">
-        <v>236</v>
-      </c>
-      <c r="C132" s="134"/>
-      <c r="D132" s="135">
-        <v>45680</v>
-      </c>
-      <c r="E132" s="136" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A133" s="138" t="s">
-        <v>238</v>
-      </c>
-      <c r="B133" s="139"/>
-      <c r="C133" s="139"/>
-      <c r="D133" s="140">
-        <v>46045</v>
-      </c>
-      <c r="E133" s="141" t="s">
+      <c r="E133" s="136" t="s">
         <v>239</v>
       </c>
     </row>
@@ -3764,1205 +3782,1576 @@
       <c r="E134" s="72"/>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A135" s="61" t="s">
+      <c r="A135" s="124" t="s">
         <v>9</v>
       </c>
-      <c r="B135" s="2" t="s">
+      <c r="B135" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="C135" s="2" t="s">
+      <c r="C135" s="50" t="s">
         <v>135</v>
       </c>
-      <c r="D135" s="66">
+      <c r="D135" s="67">
         <v>46052</v>
       </c>
       <c r="E135" s="72"/>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A136" s="61" t="s">
+      <c r="A136" s="124" t="s">
         <v>194</v>
       </c>
-      <c r="B136" s="2" t="s">
+      <c r="B136" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="C136" s="2" t="s">
+      <c r="C136" s="50" t="s">
         <v>151</v>
       </c>
-      <c r="D136" s="66">
+      <c r="D136" s="67">
         <v>46054</v>
       </c>
       <c r="E136" s="72"/>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A137" s="60" t="s">
+      <c r="A137" s="62" t="s">
+        <v>89</v>
+      </c>
+      <c r="B137" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="C137" s="50" t="s">
+        <v>155</v>
+      </c>
+      <c r="D137" s="67">
+        <v>46062</v>
+      </c>
+      <c r="E137" s="72"/>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A138" s="60" t="s">
+        <v>50</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="C138" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D138" s="66">
+        <v>46062</v>
+      </c>
+      <c r="E138" s="72"/>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A139" s="60" t="s">
+        <v>49</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="C139" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D139" s="66">
+        <v>46065</v>
+      </c>
+      <c r="E139" s="72"/>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A140" s="62" t="s">
         <v>246</v>
       </c>
-      <c r="B137" s="2" t="s">
+      <c r="B140" s="50" t="s">
         <v>247</v>
       </c>
-      <c r="C137" s="2" t="s">
+      <c r="C140" s="50" t="s">
         <v>248</v>
       </c>
-      <c r="D137" s="66">
+      <c r="D140" s="67">
         <v>46065</v>
       </c>
-      <c r="E137" s="72"/>
-    </row>
-    <row r="138" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A138" s="112" t="s">
+      <c r="E140" s="72"/>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A141" s="135" t="s">
+        <v>249</v>
+      </c>
+      <c r="B141" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="C141" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="D141" s="66">
+        <v>46069</v>
+      </c>
+      <c r="E141" s="72"/>
+    </row>
+    <row r="142" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A142" s="112" t="s">
         <v>13</v>
       </c>
-      <c r="B138" s="117" t="s">
+      <c r="B142" s="117" t="s">
         <v>180</v>
       </c>
-      <c r="C138" s="117" t="s">
+      <c r="C142" s="117" t="s">
         <v>111</v>
       </c>
-      <c r="D138" s="118">
+      <c r="D142" s="118">
         <v>46070</v>
       </c>
-      <c r="E138" s="116" t="s">
+      <c r="E142" s="116" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A139" s="112" t="s">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A143" s="112" t="s">
         <v>63</v>
       </c>
-      <c r="B139" s="113" t="s">
+      <c r="B143" s="113" t="s">
         <v>178</v>
       </c>
-      <c r="C139" s="113" t="s">
+      <c r="C143" s="113" t="s">
         <v>187</v>
       </c>
-      <c r="D139" s="114">
+      <c r="D143" s="114">
         <v>46084</v>
       </c>
-      <c r="E139" s="115" t="s">
+      <c r="E143" s="115" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A140" s="60" t="s">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A144" s="60" t="s">
         <v>192</v>
       </c>
-      <c r="B140" s="2" t="s">
+      <c r="B144" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="C140" s="2" t="s">
+      <c r="C144" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="D140" s="66">
+      <c r="D144" s="66">
         <v>46092</v>
       </c>
-      <c r="E140" s="72"/>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A141" s="61" t="s">
+      <c r="E144" s="72"/>
+    </row>
+    <row r="145" spans="1:122" x14ac:dyDescent="0.35">
+      <c r="A145" s="124" t="s">
         <v>18</v>
       </c>
-      <c r="B141" s="2" t="s">
+      <c r="B145" s="50" t="s">
         <v>228</v>
       </c>
-      <c r="C141" s="2" t="s">
+      <c r="C145" s="50" t="s">
         <v>230</v>
       </c>
-      <c r="D141" s="66">
+      <c r="D145" s="67">
         <v>46093</v>
       </c>
-      <c r="E141" s="72"/>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A142" s="60" t="s">
+      <c r="E145" s="72"/>
+    </row>
+    <row r="146" spans="1:122" x14ac:dyDescent="0.35">
+      <c r="A146" s="60" t="s">
         <v>192</v>
       </c>
-      <c r="B142" s="2" t="s">
+      <c r="B146" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="C142" s="2" t="s">
+      <c r="C146" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="D142" s="66">
+      <c r="D146" s="66">
         <v>46094</v>
       </c>
-      <c r="E142" s="72"/>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A143" s="61" t="s">
-        <v>55</v>
-      </c>
-      <c r="B143" s="2"/>
-      <c r="C143" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D143" s="66">
-        <v>46109</v>
-      </c>
-      <c r="E143" s="72"/>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A144" s="61" t="s">
-        <v>9</v>
-      </c>
-      <c r="B144" s="2"/>
-      <c r="C144" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D144" s="69">
-        <v>46113</v>
-      </c>
-      <c r="E144" s="72"/>
-    </row>
-    <row r="145" spans="1:122" x14ac:dyDescent="0.35">
-      <c r="A145" s="60" t="s">
-        <v>17</v>
-      </c>
-      <c r="B145" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="C145" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="D145" s="69">
-        <v>46118</v>
-      </c>
-      <c r="E145" s="72"/>
-    </row>
-    <row r="146" spans="1:122" x14ac:dyDescent="0.35">
-      <c r="A146" s="61" t="s">
-        <v>36</v>
-      </c>
-      <c r="B146" s="2"/>
-      <c r="C146" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D146" s="69">
-        <v>46165</v>
-      </c>
       <c r="E146" s="72"/>
     </row>
     <row r="147" spans="1:122" x14ac:dyDescent="0.35">
-      <c r="A147" s="61" t="s">
-        <v>30</v>
-      </c>
-      <c r="B147" s="1"/>
+      <c r="A147" s="60" t="s">
+        <v>66</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>253</v>
+      </c>
       <c r="C147" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D147" s="69">
-        <v>46167</v>
-      </c>
-      <c r="E147" s="72"/>
+        <v>219</v>
+      </c>
+      <c r="D147" s="66">
+        <v>46104</v>
+      </c>
+      <c r="E147" s="141" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="148" spans="1:122" x14ac:dyDescent="0.35">
       <c r="A148" s="61" t="s">
-        <v>53</v>
-      </c>
-      <c r="B148" s="1"/>
+        <v>55</v>
+      </c>
+      <c r="B148" s="2"/>
       <c r="C148" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D148" s="69">
-        <v>46167</v>
+      <c r="D148" s="66">
+        <v>46109</v>
       </c>
       <c r="E148" s="72"/>
     </row>
     <row r="149" spans="1:122" x14ac:dyDescent="0.35">
       <c r="A149" s="61" t="s">
+        <v>9</v>
+      </c>
+      <c r="B149" s="2"/>
+      <c r="C149" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D149" s="69">
+        <v>46113</v>
+      </c>
+      <c r="E149" s="72"/>
+    </row>
+    <row r="150" spans="1:122" x14ac:dyDescent="0.35">
+      <c r="A150" s="60" t="s">
+        <v>17</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C150" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D150" s="69">
+        <v>46118</v>
+      </c>
+      <c r="E150" s="72"/>
+    </row>
+    <row r="151" spans="1:122" x14ac:dyDescent="0.35">
+      <c r="A151" s="61" t="s">
+        <v>36</v>
+      </c>
+      <c r="B151" s="2"/>
+      <c r="C151" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D151" s="69">
+        <v>46165</v>
+      </c>
+      <c r="E151" s="72"/>
+    </row>
+    <row r="152" spans="1:122" x14ac:dyDescent="0.35">
+      <c r="A152" s="61" t="s">
+        <v>30</v>
+      </c>
+      <c r="B152" s="1"/>
+      <c r="C152" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D152" s="69">
+        <v>46167</v>
+      </c>
+      <c r="E152" s="72"/>
+    </row>
+    <row r="153" spans="1:122" x14ac:dyDescent="0.35">
+      <c r="A153" s="61" t="s">
+        <v>53</v>
+      </c>
+      <c r="B153" s="1"/>
+      <c r="C153" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D153" s="69">
+        <v>46167</v>
+      </c>
+      <c r="E153" s="72"/>
+    </row>
+    <row r="154" spans="1:122" x14ac:dyDescent="0.35">
+      <c r="A154" s="61" t="s">
         <v>231</v>
       </c>
-      <c r="B149" s="1" t="s">
+      <c r="B154" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="C149" s="2" t="s">
+      <c r="C154" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="D149" s="69">
+      <c r="D154" s="69">
         <v>46184</v>
       </c>
-      <c r="E149" s="72"/>
-    </row>
-    <row r="150" spans="1:122" x14ac:dyDescent="0.35">
-      <c r="A150" s="61" t="s">
-        <v>192</v>
-      </c>
-      <c r="B150" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="C150" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="D150" s="69">
-        <v>46184</v>
-      </c>
-      <c r="E150" s="72"/>
-    </row>
-    <row r="151" spans="1:122" s="54" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A151" s="112" t="s">
-        <v>63</v>
-      </c>
-      <c r="B151" s="113" t="s">
-        <v>64</v>
-      </c>
-      <c r="C151" s="113" t="s">
-        <v>14</v>
-      </c>
-      <c r="D151" s="119">
-        <v>46194</v>
-      </c>
-      <c r="E151" s="115" t="s">
-        <v>213</v>
-      </c>
-      <c r="F151"/>
-      <c r="G151"/>
-      <c r="H151"/>
-      <c r="I151"/>
-      <c r="J151"/>
-      <c r="K151"/>
-      <c r="L151"/>
-      <c r="M151"/>
-      <c r="N151"/>
-      <c r="O151"/>
-      <c r="P151"/>
-      <c r="Q151"/>
-      <c r="R151"/>
-      <c r="S151"/>
-      <c r="T151"/>
-      <c r="U151"/>
-      <c r="V151"/>
-      <c r="W151"/>
-      <c r="X151"/>
-      <c r="Y151"/>
-      <c r="Z151"/>
-      <c r="AA151"/>
-      <c r="AB151"/>
-      <c r="AC151"/>
-      <c r="AD151"/>
-      <c r="AE151"/>
-      <c r="AF151"/>
-      <c r="AG151"/>
-      <c r="AH151"/>
-      <c r="AI151"/>
-      <c r="AJ151"/>
-      <c r="AK151"/>
-      <c r="AL151"/>
-      <c r="AM151"/>
-      <c r="AN151"/>
-      <c r="AO151"/>
-      <c r="AP151"/>
-      <c r="AQ151"/>
-      <c r="AR151"/>
-      <c r="AS151"/>
-      <c r="AT151"/>
-      <c r="AU151"/>
-      <c r="AV151"/>
-      <c r="AW151"/>
-      <c r="AX151"/>
-      <c r="AY151"/>
-      <c r="AZ151"/>
-      <c r="BA151"/>
-      <c r="BB151"/>
-      <c r="BC151"/>
-      <c r="BD151"/>
-      <c r="BE151"/>
-      <c r="BF151"/>
-      <c r="BG151"/>
-      <c r="BH151"/>
-      <c r="BI151"/>
-      <c r="BJ151"/>
-      <c r="BK151"/>
-      <c r="BL151"/>
-      <c r="BM151"/>
-      <c r="BN151"/>
-      <c r="BO151"/>
-      <c r="BP151"/>
-      <c r="BQ151"/>
-      <c r="BR151"/>
-      <c r="BS151"/>
-      <c r="BT151"/>
-      <c r="BU151"/>
-      <c r="BV151"/>
-      <c r="BW151"/>
-      <c r="BX151"/>
-      <c r="BY151"/>
-      <c r="BZ151"/>
-      <c r="CA151"/>
-      <c r="CB151"/>
-      <c r="CC151"/>
-      <c r="CD151"/>
-      <c r="CE151"/>
-      <c r="CF151"/>
-      <c r="CG151"/>
-      <c r="CH151"/>
-      <c r="CI151"/>
-      <c r="CJ151"/>
-      <c r="CK151"/>
-      <c r="CL151"/>
-      <c r="CM151"/>
-      <c r="CN151"/>
-      <c r="CO151"/>
-      <c r="CP151"/>
-      <c r="CQ151"/>
-      <c r="CR151"/>
-      <c r="CS151"/>
-      <c r="CT151"/>
-      <c r="CU151"/>
-      <c r="CV151"/>
-      <c r="CW151"/>
-      <c r="CX151"/>
-      <c r="CY151"/>
-      <c r="CZ151"/>
-      <c r="DA151"/>
-      <c r="DB151"/>
-      <c r="DC151"/>
-      <c r="DD151"/>
-      <c r="DE151"/>
-      <c r="DF151"/>
-      <c r="DG151"/>
-      <c r="DH151"/>
-      <c r="DI151"/>
-      <c r="DJ151"/>
-      <c r="DK151"/>
-      <c r="DL151"/>
-      <c r="DM151"/>
-      <c r="DN151"/>
-      <c r="DO151"/>
-      <c r="DP151"/>
-      <c r="DQ151"/>
-      <c r="DR151"/>
-    </row>
-    <row r="152" spans="1:122" s="54" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A152" s="112" t="s">
-        <v>241</v>
-      </c>
-      <c r="B152" s="113" t="s">
-        <v>242</v>
-      </c>
-      <c r="C152" s="113" t="s">
-        <v>243</v>
-      </c>
-      <c r="D152" s="119">
-        <v>46205</v>
-      </c>
-      <c r="E152" s="115"/>
-      <c r="F152"/>
-      <c r="G152"/>
-      <c r="H152"/>
-      <c r="I152"/>
-      <c r="J152"/>
-      <c r="K152"/>
-      <c r="L152"/>
-      <c r="M152"/>
-      <c r="N152"/>
-      <c r="O152"/>
-      <c r="P152"/>
-      <c r="Q152"/>
-      <c r="R152"/>
-      <c r="S152"/>
-      <c r="T152"/>
-      <c r="U152"/>
-      <c r="V152"/>
-      <c r="W152"/>
-      <c r="X152"/>
-      <c r="Y152"/>
-      <c r="Z152"/>
-      <c r="AA152"/>
-      <c r="AB152"/>
-      <c r="AC152"/>
-      <c r="AD152"/>
-      <c r="AE152"/>
-      <c r="AF152"/>
-      <c r="AG152"/>
-      <c r="AH152"/>
-      <c r="AI152"/>
-      <c r="AJ152"/>
-      <c r="AK152"/>
-      <c r="AL152"/>
-      <c r="AM152"/>
-      <c r="AN152"/>
-      <c r="AO152"/>
-      <c r="AP152"/>
-      <c r="AQ152"/>
-      <c r="AR152"/>
-      <c r="AS152"/>
-      <c r="AT152"/>
-      <c r="AU152"/>
-      <c r="AV152"/>
-      <c r="AW152"/>
-      <c r="AX152"/>
-      <c r="AY152"/>
-      <c r="AZ152"/>
-      <c r="BA152"/>
-      <c r="BB152"/>
-      <c r="BC152"/>
-      <c r="BD152"/>
-      <c r="BE152"/>
-      <c r="BF152"/>
-      <c r="BG152"/>
-      <c r="BH152"/>
-      <c r="BI152"/>
-      <c r="BJ152"/>
-      <c r="BK152"/>
-      <c r="BL152"/>
-      <c r="BM152"/>
-      <c r="BN152"/>
-      <c r="BO152"/>
-      <c r="BP152"/>
-      <c r="BQ152"/>
-      <c r="BR152"/>
-      <c r="BS152"/>
-      <c r="BT152"/>
-      <c r="BU152"/>
-      <c r="BV152"/>
-      <c r="BW152"/>
-      <c r="BX152"/>
-      <c r="BY152"/>
-      <c r="BZ152"/>
-      <c r="CA152"/>
-      <c r="CB152"/>
-      <c r="CC152"/>
-      <c r="CD152"/>
-      <c r="CE152"/>
-      <c r="CF152"/>
-      <c r="CG152"/>
-      <c r="CH152"/>
-      <c r="CI152"/>
-      <c r="CJ152"/>
-      <c r="CK152"/>
-      <c r="CL152"/>
-      <c r="CM152"/>
-      <c r="CN152"/>
-      <c r="CO152"/>
-      <c r="CP152"/>
-      <c r="CQ152"/>
-      <c r="CR152"/>
-      <c r="CS152"/>
-      <c r="CT152"/>
-      <c r="CU152"/>
-      <c r="CV152"/>
-      <c r="CW152"/>
-      <c r="CX152"/>
-      <c r="CY152"/>
-      <c r="CZ152"/>
-      <c r="DA152"/>
-      <c r="DB152"/>
-      <c r="DC152"/>
-      <c r="DD152"/>
-      <c r="DE152"/>
-      <c r="DF152"/>
-      <c r="DG152"/>
-      <c r="DH152"/>
-      <c r="DI152"/>
-      <c r="DJ152"/>
-      <c r="DK152"/>
-      <c r="DL152"/>
-      <c r="DM152"/>
-      <c r="DN152"/>
-      <c r="DO152"/>
-      <c r="DP152"/>
-      <c r="DQ152"/>
-      <c r="DR152"/>
-    </row>
-    <row r="153" spans="1:122" s="54" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A153" s="112" t="s">
-        <v>244</v>
-      </c>
-      <c r="B153" s="113" t="s">
-        <v>242</v>
-      </c>
-      <c r="C153" s="113" t="s">
-        <v>243</v>
-      </c>
-      <c r="D153" s="119">
-        <v>46205</v>
-      </c>
-      <c r="E153" s="115"/>
-      <c r="F153"/>
-      <c r="G153"/>
-      <c r="H153"/>
-      <c r="I153"/>
-      <c r="J153"/>
-      <c r="K153"/>
-      <c r="L153"/>
-      <c r="M153"/>
-      <c r="N153"/>
-      <c r="O153"/>
-      <c r="P153"/>
-      <c r="Q153"/>
-      <c r="R153"/>
-      <c r="S153"/>
-      <c r="T153"/>
-      <c r="U153"/>
-      <c r="V153"/>
-      <c r="W153"/>
-      <c r="X153"/>
-      <c r="Y153"/>
-      <c r="Z153"/>
-      <c r="AA153"/>
-      <c r="AB153"/>
-      <c r="AC153"/>
-      <c r="AD153"/>
-      <c r="AE153"/>
-      <c r="AF153"/>
-      <c r="AG153"/>
-      <c r="AH153"/>
-      <c r="AI153"/>
-      <c r="AJ153"/>
-      <c r="AK153"/>
-      <c r="AL153"/>
-      <c r="AM153"/>
-      <c r="AN153"/>
-      <c r="AO153"/>
-      <c r="AP153"/>
-      <c r="AQ153"/>
-      <c r="AR153"/>
-      <c r="AS153"/>
-      <c r="AT153"/>
-      <c r="AU153"/>
-      <c r="AV153"/>
-      <c r="AW153"/>
-      <c r="AX153"/>
-      <c r="AY153"/>
-      <c r="AZ153"/>
-      <c r="BA153"/>
-      <c r="BB153"/>
-      <c r="BC153"/>
-      <c r="BD153"/>
-      <c r="BE153"/>
-      <c r="BF153"/>
-      <c r="BG153"/>
-      <c r="BH153"/>
-      <c r="BI153"/>
-      <c r="BJ153"/>
-      <c r="BK153"/>
-      <c r="BL153"/>
-      <c r="BM153"/>
-      <c r="BN153"/>
-      <c r="BO153"/>
-      <c r="BP153"/>
-      <c r="BQ153"/>
-      <c r="BR153"/>
-      <c r="BS153"/>
-      <c r="BT153"/>
-      <c r="BU153"/>
-      <c r="BV153"/>
-      <c r="BW153"/>
-      <c r="BX153"/>
-      <c r="BY153"/>
-      <c r="BZ153"/>
-      <c r="CA153"/>
-      <c r="CB153"/>
-      <c r="CC153"/>
-      <c r="CD153"/>
-      <c r="CE153"/>
-      <c r="CF153"/>
-      <c r="CG153"/>
-      <c r="CH153"/>
-      <c r="CI153"/>
-      <c r="CJ153"/>
-      <c r="CK153"/>
-      <c r="CL153"/>
-      <c r="CM153"/>
-      <c r="CN153"/>
-      <c r="CO153"/>
-      <c r="CP153"/>
-      <c r="CQ153"/>
-      <c r="CR153"/>
-      <c r="CS153"/>
-      <c r="CT153"/>
-      <c r="CU153"/>
-      <c r="CV153"/>
-      <c r="CW153"/>
-      <c r="CX153"/>
-      <c r="CY153"/>
-      <c r="CZ153"/>
-      <c r="DA153"/>
-      <c r="DB153"/>
-      <c r="DC153"/>
-      <c r="DD153"/>
-      <c r="DE153"/>
-      <c r="DF153"/>
-      <c r="DG153"/>
-      <c r="DH153"/>
-      <c r="DI153"/>
-      <c r="DJ153"/>
-      <c r="DK153"/>
-      <c r="DL153"/>
-      <c r="DM153"/>
-      <c r="DN153"/>
-      <c r="DO153"/>
-      <c r="DP153"/>
-      <c r="DQ153"/>
-      <c r="DR153"/>
-    </row>
-    <row r="154" spans="1:122" s="55" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A154" s="64" t="s">
-        <v>5</v>
-      </c>
-      <c r="B154" s="43" t="s">
-        <v>125</v>
-      </c>
-      <c r="C154" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="D154" s="70">
-        <v>46220</v>
-      </c>
-      <c r="E154" s="75"/>
-      <c r="F154"/>
-      <c r="G154"/>
-      <c r="H154"/>
-      <c r="I154"/>
-      <c r="J154"/>
-      <c r="K154"/>
-      <c r="L154"/>
-      <c r="M154"/>
-      <c r="N154"/>
-      <c r="O154"/>
-      <c r="P154"/>
-      <c r="Q154"/>
-      <c r="R154"/>
-      <c r="S154"/>
-      <c r="T154"/>
-      <c r="U154"/>
-      <c r="V154"/>
-      <c r="W154"/>
-      <c r="X154"/>
-      <c r="Y154"/>
-      <c r="Z154"/>
-      <c r="AA154"/>
-      <c r="AB154"/>
-      <c r="AC154"/>
-      <c r="AD154"/>
-      <c r="AE154"/>
-      <c r="AF154"/>
-      <c r="AG154"/>
-      <c r="AH154"/>
-      <c r="AI154"/>
-      <c r="AJ154"/>
-      <c r="AK154"/>
-      <c r="AL154"/>
-      <c r="AM154"/>
-      <c r="AN154"/>
-      <c r="AO154"/>
-      <c r="AP154"/>
-      <c r="AQ154"/>
-      <c r="AR154"/>
-      <c r="AS154"/>
-      <c r="AT154"/>
-      <c r="AU154"/>
-      <c r="AV154"/>
-      <c r="AW154"/>
-      <c r="AX154"/>
-      <c r="AY154"/>
-      <c r="AZ154"/>
-      <c r="BA154"/>
-      <c r="BB154"/>
-      <c r="BC154"/>
-      <c r="BD154"/>
-      <c r="BE154"/>
-      <c r="BF154"/>
-      <c r="BG154"/>
-      <c r="BH154"/>
-      <c r="BI154"/>
-      <c r="BJ154"/>
-      <c r="BK154"/>
-      <c r="BL154"/>
-      <c r="BM154"/>
-      <c r="BN154"/>
-      <c r="BO154"/>
-      <c r="BP154"/>
-      <c r="BQ154"/>
-      <c r="BR154"/>
-      <c r="BS154"/>
-      <c r="BT154"/>
-      <c r="BU154"/>
-      <c r="BV154"/>
-      <c r="BW154"/>
-      <c r="BX154"/>
-      <c r="BY154"/>
-      <c r="BZ154"/>
-      <c r="CA154"/>
-      <c r="CB154"/>
-      <c r="CC154"/>
-      <c r="CD154"/>
-      <c r="CE154"/>
-      <c r="CF154"/>
-      <c r="CG154"/>
-      <c r="CH154"/>
-      <c r="CI154"/>
-      <c r="CJ154"/>
-      <c r="CK154"/>
-      <c r="CL154"/>
-      <c r="CM154"/>
-      <c r="CN154"/>
-      <c r="CO154"/>
-      <c r="CP154"/>
-      <c r="CQ154"/>
-      <c r="CR154"/>
-      <c r="CS154"/>
-      <c r="CT154"/>
-      <c r="CU154"/>
-      <c r="CV154"/>
-      <c r="CW154"/>
-      <c r="CX154"/>
-      <c r="CY154"/>
-      <c r="CZ154"/>
-      <c r="DA154"/>
-      <c r="DB154"/>
-      <c r="DC154"/>
-      <c r="DD154"/>
-      <c r="DE154"/>
-      <c r="DF154"/>
-      <c r="DG154"/>
-      <c r="DH154"/>
-      <c r="DI154"/>
-      <c r="DJ154"/>
-      <c r="DK154"/>
-      <c r="DL154"/>
-      <c r="DM154"/>
-      <c r="DN154"/>
-      <c r="DO154"/>
-      <c r="DP154"/>
-      <c r="DQ154"/>
-      <c r="DR154"/>
+      <c r="E154" s="72"/>
     </row>
     <row r="155" spans="1:122" x14ac:dyDescent="0.35">
       <c r="A155" s="61" t="s">
+        <v>192</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C155" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="D155" s="69">
+        <v>46184</v>
+      </c>
+      <c r="E155" s="72"/>
+    </row>
+    <row r="156" spans="1:122" s="54" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A156" s="112" t="s">
+        <v>63</v>
+      </c>
+      <c r="B156" s="113" t="s">
+        <v>64</v>
+      </c>
+      <c r="C156" s="113" t="s">
+        <v>14</v>
+      </c>
+      <c r="D156" s="119">
+        <v>46194</v>
+      </c>
+      <c r="E156" s="115" t="s">
+        <v>213</v>
+      </c>
+      <c r="F156"/>
+      <c r="G156"/>
+      <c r="H156"/>
+      <c r="I156"/>
+      <c r="J156"/>
+      <c r="K156"/>
+      <c r="L156"/>
+      <c r="M156"/>
+      <c r="N156"/>
+      <c r="O156"/>
+      <c r="P156"/>
+      <c r="Q156"/>
+      <c r="R156"/>
+      <c r="S156"/>
+      <c r="T156"/>
+      <c r="U156"/>
+      <c r="V156"/>
+      <c r="W156"/>
+      <c r="X156"/>
+      <c r="Y156"/>
+      <c r="Z156"/>
+      <c r="AA156"/>
+      <c r="AB156"/>
+      <c r="AC156"/>
+      <c r="AD156"/>
+      <c r="AE156"/>
+      <c r="AF156"/>
+      <c r="AG156"/>
+      <c r="AH156"/>
+      <c r="AI156"/>
+      <c r="AJ156"/>
+      <c r="AK156"/>
+      <c r="AL156"/>
+      <c r="AM156"/>
+      <c r="AN156"/>
+      <c r="AO156"/>
+      <c r="AP156"/>
+      <c r="AQ156"/>
+      <c r="AR156"/>
+      <c r="AS156"/>
+      <c r="AT156"/>
+      <c r="AU156"/>
+      <c r="AV156"/>
+      <c r="AW156"/>
+      <c r="AX156"/>
+      <c r="AY156"/>
+      <c r="AZ156"/>
+      <c r="BA156"/>
+      <c r="BB156"/>
+      <c r="BC156"/>
+      <c r="BD156"/>
+      <c r="BE156"/>
+      <c r="BF156"/>
+      <c r="BG156"/>
+      <c r="BH156"/>
+      <c r="BI156"/>
+      <c r="BJ156"/>
+      <c r="BK156"/>
+      <c r="BL156"/>
+      <c r="BM156"/>
+      <c r="BN156"/>
+      <c r="BO156"/>
+      <c r="BP156"/>
+      <c r="BQ156"/>
+      <c r="BR156"/>
+      <c r="BS156"/>
+      <c r="BT156"/>
+      <c r="BU156"/>
+      <c r="BV156"/>
+      <c r="BW156"/>
+      <c r="BX156"/>
+      <c r="BY156"/>
+      <c r="BZ156"/>
+      <c r="CA156"/>
+      <c r="CB156"/>
+      <c r="CC156"/>
+      <c r="CD156"/>
+      <c r="CE156"/>
+      <c r="CF156"/>
+      <c r="CG156"/>
+      <c r="CH156"/>
+      <c r="CI156"/>
+      <c r="CJ156"/>
+      <c r="CK156"/>
+      <c r="CL156"/>
+      <c r="CM156"/>
+      <c r="CN156"/>
+      <c r="CO156"/>
+      <c r="CP156"/>
+      <c r="CQ156"/>
+      <c r="CR156"/>
+      <c r="CS156"/>
+      <c r="CT156"/>
+      <c r="CU156"/>
+      <c r="CV156"/>
+      <c r="CW156"/>
+      <c r="CX156"/>
+      <c r="CY156"/>
+      <c r="CZ156"/>
+      <c r="DA156"/>
+      <c r="DB156"/>
+      <c r="DC156"/>
+      <c r="DD156"/>
+      <c r="DE156"/>
+      <c r="DF156"/>
+      <c r="DG156"/>
+      <c r="DH156"/>
+      <c r="DI156"/>
+      <c r="DJ156"/>
+      <c r="DK156"/>
+      <c r="DL156"/>
+      <c r="DM156"/>
+      <c r="DN156"/>
+      <c r="DO156"/>
+      <c r="DP156"/>
+      <c r="DQ156"/>
+      <c r="DR156"/>
+    </row>
+    <row r="157" spans="1:122" s="54" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A157" s="112" t="s">
+        <v>31</v>
+      </c>
+      <c r="B157" s="113" t="s">
+        <v>27</v>
+      </c>
+      <c r="C157" s="113" t="s">
+        <v>27</v>
+      </c>
+      <c r="D157" s="119">
+        <v>46203</v>
+      </c>
+      <c r="E157" s="115"/>
+      <c r="F157"/>
+      <c r="G157"/>
+      <c r="H157"/>
+      <c r="I157"/>
+      <c r="J157"/>
+      <c r="K157"/>
+      <c r="L157"/>
+      <c r="M157"/>
+      <c r="N157"/>
+      <c r="O157"/>
+      <c r="P157"/>
+      <c r="Q157"/>
+      <c r="R157"/>
+      <c r="S157"/>
+      <c r="T157"/>
+      <c r="U157"/>
+      <c r="V157"/>
+      <c r="W157"/>
+      <c r="X157"/>
+      <c r="Y157"/>
+      <c r="Z157"/>
+      <c r="AA157"/>
+      <c r="AB157"/>
+      <c r="AC157"/>
+      <c r="AD157"/>
+      <c r="AE157"/>
+      <c r="AF157"/>
+      <c r="AG157"/>
+      <c r="AH157"/>
+      <c r="AI157"/>
+      <c r="AJ157"/>
+      <c r="AK157"/>
+      <c r="AL157"/>
+      <c r="AM157"/>
+      <c r="AN157"/>
+      <c r="AO157"/>
+      <c r="AP157"/>
+      <c r="AQ157"/>
+      <c r="AR157"/>
+      <c r="AS157"/>
+      <c r="AT157"/>
+      <c r="AU157"/>
+      <c r="AV157"/>
+      <c r="AW157"/>
+      <c r="AX157"/>
+      <c r="AY157"/>
+      <c r="AZ157"/>
+      <c r="BA157"/>
+      <c r="BB157"/>
+      <c r="BC157"/>
+      <c r="BD157"/>
+      <c r="BE157"/>
+      <c r="BF157"/>
+      <c r="BG157"/>
+      <c r="BH157"/>
+      <c r="BI157"/>
+      <c r="BJ157"/>
+      <c r="BK157"/>
+      <c r="BL157"/>
+      <c r="BM157"/>
+      <c r="BN157"/>
+      <c r="BO157"/>
+      <c r="BP157"/>
+      <c r="BQ157"/>
+      <c r="BR157"/>
+      <c r="BS157"/>
+      <c r="BT157"/>
+      <c r="BU157"/>
+      <c r="BV157"/>
+      <c r="BW157"/>
+      <c r="BX157"/>
+      <c r="BY157"/>
+      <c r="BZ157"/>
+      <c r="CA157"/>
+      <c r="CB157"/>
+      <c r="CC157"/>
+      <c r="CD157"/>
+      <c r="CE157"/>
+      <c r="CF157"/>
+      <c r="CG157"/>
+      <c r="CH157"/>
+      <c r="CI157"/>
+      <c r="CJ157"/>
+      <c r="CK157"/>
+      <c r="CL157"/>
+      <c r="CM157"/>
+      <c r="CN157"/>
+      <c r="CO157"/>
+      <c r="CP157"/>
+      <c r="CQ157"/>
+      <c r="CR157"/>
+      <c r="CS157"/>
+      <c r="CT157"/>
+      <c r="CU157"/>
+      <c r="CV157"/>
+      <c r="CW157"/>
+      <c r="CX157"/>
+      <c r="CY157"/>
+      <c r="CZ157"/>
+      <c r="DA157"/>
+      <c r="DB157"/>
+      <c r="DC157"/>
+      <c r="DD157"/>
+      <c r="DE157"/>
+      <c r="DF157"/>
+      <c r="DG157"/>
+      <c r="DH157"/>
+      <c r="DI157"/>
+      <c r="DJ157"/>
+      <c r="DK157"/>
+      <c r="DL157"/>
+      <c r="DM157"/>
+      <c r="DN157"/>
+      <c r="DO157"/>
+      <c r="DP157"/>
+      <c r="DQ157"/>
+      <c r="DR157"/>
+    </row>
+    <row r="158" spans="1:122" s="54" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A158" s="112" t="s">
+        <v>241</v>
+      </c>
+      <c r="B158" s="113" t="s">
+        <v>242</v>
+      </c>
+      <c r="C158" s="113" t="s">
+        <v>243</v>
+      </c>
+      <c r="D158" s="119">
+        <v>46205</v>
+      </c>
+      <c r="E158" s="115"/>
+      <c r="F158"/>
+      <c r="G158"/>
+      <c r="H158"/>
+      <c r="I158"/>
+      <c r="J158"/>
+      <c r="K158"/>
+      <c r="L158"/>
+      <c r="M158"/>
+      <c r="N158"/>
+      <c r="O158"/>
+      <c r="P158"/>
+      <c r="Q158"/>
+      <c r="R158"/>
+      <c r="S158"/>
+      <c r="T158"/>
+      <c r="U158"/>
+      <c r="V158"/>
+      <c r="W158"/>
+      <c r="X158"/>
+      <c r="Y158"/>
+      <c r="Z158"/>
+      <c r="AA158"/>
+      <c r="AB158"/>
+      <c r="AC158"/>
+      <c r="AD158"/>
+      <c r="AE158"/>
+      <c r="AF158"/>
+      <c r="AG158"/>
+      <c r="AH158"/>
+      <c r="AI158"/>
+      <c r="AJ158"/>
+      <c r="AK158"/>
+      <c r="AL158"/>
+      <c r="AM158"/>
+      <c r="AN158"/>
+      <c r="AO158"/>
+      <c r="AP158"/>
+      <c r="AQ158"/>
+      <c r="AR158"/>
+      <c r="AS158"/>
+      <c r="AT158"/>
+      <c r="AU158"/>
+      <c r="AV158"/>
+      <c r="AW158"/>
+      <c r="AX158"/>
+      <c r="AY158"/>
+      <c r="AZ158"/>
+      <c r="BA158"/>
+      <c r="BB158"/>
+      <c r="BC158"/>
+      <c r="BD158"/>
+      <c r="BE158"/>
+      <c r="BF158"/>
+      <c r="BG158"/>
+      <c r="BH158"/>
+      <c r="BI158"/>
+      <c r="BJ158"/>
+      <c r="BK158"/>
+      <c r="BL158"/>
+      <c r="BM158"/>
+      <c r="BN158"/>
+      <c r="BO158"/>
+      <c r="BP158"/>
+      <c r="BQ158"/>
+      <c r="BR158"/>
+      <c r="BS158"/>
+      <c r="BT158"/>
+      <c r="BU158"/>
+      <c r="BV158"/>
+      <c r="BW158"/>
+      <c r="BX158"/>
+      <c r="BY158"/>
+      <c r="BZ158"/>
+      <c r="CA158"/>
+      <c r="CB158"/>
+      <c r="CC158"/>
+      <c r="CD158"/>
+      <c r="CE158"/>
+      <c r="CF158"/>
+      <c r="CG158"/>
+      <c r="CH158"/>
+      <c r="CI158"/>
+      <c r="CJ158"/>
+      <c r="CK158"/>
+      <c r="CL158"/>
+      <c r="CM158"/>
+      <c r="CN158"/>
+      <c r="CO158"/>
+      <c r="CP158"/>
+      <c r="CQ158"/>
+      <c r="CR158"/>
+      <c r="CS158"/>
+      <c r="CT158"/>
+      <c r="CU158"/>
+      <c r="CV158"/>
+      <c r="CW158"/>
+      <c r="CX158"/>
+      <c r="CY158"/>
+      <c r="CZ158"/>
+      <c r="DA158"/>
+      <c r="DB158"/>
+      <c r="DC158"/>
+      <c r="DD158"/>
+      <c r="DE158"/>
+      <c r="DF158"/>
+      <c r="DG158"/>
+      <c r="DH158"/>
+      <c r="DI158"/>
+      <c r="DJ158"/>
+      <c r="DK158"/>
+      <c r="DL158"/>
+      <c r="DM158"/>
+      <c r="DN158"/>
+      <c r="DO158"/>
+      <c r="DP158"/>
+      <c r="DQ158"/>
+      <c r="DR158"/>
+    </row>
+    <row r="159" spans="1:122" s="54" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A159" s="112" t="s">
+        <v>244</v>
+      </c>
+      <c r="B159" s="113" t="s">
+        <v>242</v>
+      </c>
+      <c r="C159" s="113" t="s">
+        <v>243</v>
+      </c>
+      <c r="D159" s="119">
+        <v>46205</v>
+      </c>
+      <c r="E159" s="115"/>
+      <c r="F159"/>
+      <c r="G159"/>
+      <c r="H159"/>
+      <c r="I159"/>
+      <c r="J159"/>
+      <c r="K159"/>
+      <c r="L159"/>
+      <c r="M159"/>
+      <c r="N159"/>
+      <c r="O159"/>
+      <c r="P159"/>
+      <c r="Q159"/>
+      <c r="R159"/>
+      <c r="S159"/>
+      <c r="T159"/>
+      <c r="U159"/>
+      <c r="V159"/>
+      <c r="W159"/>
+      <c r="X159"/>
+      <c r="Y159"/>
+      <c r="Z159"/>
+      <c r="AA159"/>
+      <c r="AB159"/>
+      <c r="AC159"/>
+      <c r="AD159"/>
+      <c r="AE159"/>
+      <c r="AF159"/>
+      <c r="AG159"/>
+      <c r="AH159"/>
+      <c r="AI159"/>
+      <c r="AJ159"/>
+      <c r="AK159"/>
+      <c r="AL159"/>
+      <c r="AM159"/>
+      <c r="AN159"/>
+      <c r="AO159"/>
+      <c r="AP159"/>
+      <c r="AQ159"/>
+      <c r="AR159"/>
+      <c r="AS159"/>
+      <c r="AT159"/>
+      <c r="AU159"/>
+      <c r="AV159"/>
+      <c r="AW159"/>
+      <c r="AX159"/>
+      <c r="AY159"/>
+      <c r="AZ159"/>
+      <c r="BA159"/>
+      <c r="BB159"/>
+      <c r="BC159"/>
+      <c r="BD159"/>
+      <c r="BE159"/>
+      <c r="BF159"/>
+      <c r="BG159"/>
+      <c r="BH159"/>
+      <c r="BI159"/>
+      <c r="BJ159"/>
+      <c r="BK159"/>
+      <c r="BL159"/>
+      <c r="BM159"/>
+      <c r="BN159"/>
+      <c r="BO159"/>
+      <c r="BP159"/>
+      <c r="BQ159"/>
+      <c r="BR159"/>
+      <c r="BS159"/>
+      <c r="BT159"/>
+      <c r="BU159"/>
+      <c r="BV159"/>
+      <c r="BW159"/>
+      <c r="BX159"/>
+      <c r="BY159"/>
+      <c r="BZ159"/>
+      <c r="CA159"/>
+      <c r="CB159"/>
+      <c r="CC159"/>
+      <c r="CD159"/>
+      <c r="CE159"/>
+      <c r="CF159"/>
+      <c r="CG159"/>
+      <c r="CH159"/>
+      <c r="CI159"/>
+      <c r="CJ159"/>
+      <c r="CK159"/>
+      <c r="CL159"/>
+      <c r="CM159"/>
+      <c r="CN159"/>
+      <c r="CO159"/>
+      <c r="CP159"/>
+      <c r="CQ159"/>
+      <c r="CR159"/>
+      <c r="CS159"/>
+      <c r="CT159"/>
+      <c r="CU159"/>
+      <c r="CV159"/>
+      <c r="CW159"/>
+      <c r="CX159"/>
+      <c r="CY159"/>
+      <c r="CZ159"/>
+      <c r="DA159"/>
+      <c r="DB159"/>
+      <c r="DC159"/>
+      <c r="DD159"/>
+      <c r="DE159"/>
+      <c r="DF159"/>
+      <c r="DG159"/>
+      <c r="DH159"/>
+      <c r="DI159"/>
+      <c r="DJ159"/>
+      <c r="DK159"/>
+      <c r="DL159"/>
+      <c r="DM159"/>
+      <c r="DN159"/>
+      <c r="DO159"/>
+      <c r="DP159"/>
+      <c r="DQ159"/>
+      <c r="DR159"/>
+    </row>
+    <row r="160" spans="1:122" s="54" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A160" s="112" t="s">
+        <v>5</v>
+      </c>
+      <c r="B160" s="113" t="s">
+        <v>19</v>
+      </c>
+      <c r="C160" s="113" t="s">
+        <v>111</v>
+      </c>
+      <c r="D160" s="119">
+        <v>46211</v>
+      </c>
+      <c r="E160" s="115"/>
+      <c r="F160"/>
+      <c r="G160"/>
+      <c r="H160"/>
+      <c r="I160"/>
+      <c r="J160"/>
+      <c r="K160"/>
+      <c r="L160"/>
+      <c r="M160"/>
+      <c r="N160"/>
+      <c r="O160"/>
+      <c r="P160"/>
+      <c r="Q160"/>
+      <c r="R160"/>
+      <c r="S160"/>
+      <c r="T160"/>
+      <c r="U160"/>
+      <c r="V160"/>
+      <c r="W160"/>
+      <c r="X160"/>
+      <c r="Y160"/>
+      <c r="Z160"/>
+      <c r="AA160"/>
+      <c r="AB160"/>
+      <c r="AC160"/>
+      <c r="AD160"/>
+      <c r="AE160"/>
+      <c r="AF160"/>
+      <c r="AG160"/>
+      <c r="AH160"/>
+      <c r="AI160"/>
+      <c r="AJ160"/>
+      <c r="AK160"/>
+      <c r="AL160"/>
+      <c r="AM160"/>
+      <c r="AN160"/>
+      <c r="AO160"/>
+      <c r="AP160"/>
+      <c r="AQ160"/>
+      <c r="AR160"/>
+      <c r="AS160"/>
+      <c r="AT160"/>
+      <c r="AU160"/>
+      <c r="AV160"/>
+      <c r="AW160"/>
+      <c r="AX160"/>
+      <c r="AY160"/>
+      <c r="AZ160"/>
+      <c r="BA160"/>
+      <c r="BB160"/>
+      <c r="BC160"/>
+      <c r="BD160"/>
+      <c r="BE160"/>
+      <c r="BF160"/>
+      <c r="BG160"/>
+      <c r="BH160"/>
+      <c r="BI160"/>
+      <c r="BJ160"/>
+      <c r="BK160"/>
+      <c r="BL160"/>
+      <c r="BM160"/>
+      <c r="BN160"/>
+      <c r="BO160"/>
+      <c r="BP160"/>
+      <c r="BQ160"/>
+      <c r="BR160"/>
+      <c r="BS160"/>
+      <c r="BT160"/>
+      <c r="BU160"/>
+      <c r="BV160"/>
+      <c r="BW160"/>
+      <c r="BX160"/>
+      <c r="BY160"/>
+      <c r="BZ160"/>
+      <c r="CA160"/>
+      <c r="CB160"/>
+      <c r="CC160"/>
+      <c r="CD160"/>
+      <c r="CE160"/>
+      <c r="CF160"/>
+      <c r="CG160"/>
+      <c r="CH160"/>
+      <c r="CI160"/>
+      <c r="CJ160"/>
+      <c r="CK160"/>
+      <c r="CL160"/>
+      <c r="CM160"/>
+      <c r="CN160"/>
+      <c r="CO160"/>
+      <c r="CP160"/>
+      <c r="CQ160"/>
+      <c r="CR160"/>
+      <c r="CS160"/>
+      <c r="CT160"/>
+      <c r="CU160"/>
+      <c r="CV160"/>
+      <c r="CW160"/>
+      <c r="CX160"/>
+      <c r="CY160"/>
+      <c r="CZ160"/>
+      <c r="DA160"/>
+      <c r="DB160"/>
+      <c r="DC160"/>
+      <c r="DD160"/>
+      <c r="DE160"/>
+      <c r="DF160"/>
+      <c r="DG160"/>
+      <c r="DH160"/>
+      <c r="DI160"/>
+      <c r="DJ160"/>
+      <c r="DK160"/>
+      <c r="DL160"/>
+      <c r="DM160"/>
+      <c r="DN160"/>
+      <c r="DO160"/>
+      <c r="DP160"/>
+      <c r="DQ160"/>
+      <c r="DR160"/>
+    </row>
+    <row r="161" spans="1:122" s="55" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A161" s="64" t="s">
+        <v>5</v>
+      </c>
+      <c r="B161" s="43" t="s">
+        <v>125</v>
+      </c>
+      <c r="C161" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="D161" s="70">
+        <v>46220</v>
+      </c>
+      <c r="E161" s="75"/>
+      <c r="F161"/>
+      <c r="G161"/>
+      <c r="H161"/>
+      <c r="I161"/>
+      <c r="J161"/>
+      <c r="K161"/>
+      <c r="L161"/>
+      <c r="M161"/>
+      <c r="N161"/>
+      <c r="O161"/>
+      <c r="P161"/>
+      <c r="Q161"/>
+      <c r="R161"/>
+      <c r="S161"/>
+      <c r="T161"/>
+      <c r="U161"/>
+      <c r="V161"/>
+      <c r="W161"/>
+      <c r="X161"/>
+      <c r="Y161"/>
+      <c r="Z161"/>
+      <c r="AA161"/>
+      <c r="AB161"/>
+      <c r="AC161"/>
+      <c r="AD161"/>
+      <c r="AE161"/>
+      <c r="AF161"/>
+      <c r="AG161"/>
+      <c r="AH161"/>
+      <c r="AI161"/>
+      <c r="AJ161"/>
+      <c r="AK161"/>
+      <c r="AL161"/>
+      <c r="AM161"/>
+      <c r="AN161"/>
+      <c r="AO161"/>
+      <c r="AP161"/>
+      <c r="AQ161"/>
+      <c r="AR161"/>
+      <c r="AS161"/>
+      <c r="AT161"/>
+      <c r="AU161"/>
+      <c r="AV161"/>
+      <c r="AW161"/>
+      <c r="AX161"/>
+      <c r="AY161"/>
+      <c r="AZ161"/>
+      <c r="BA161"/>
+      <c r="BB161"/>
+      <c r="BC161"/>
+      <c r="BD161"/>
+      <c r="BE161"/>
+      <c r="BF161"/>
+      <c r="BG161"/>
+      <c r="BH161"/>
+      <c r="BI161"/>
+      <c r="BJ161"/>
+      <c r="BK161"/>
+      <c r="BL161"/>
+      <c r="BM161"/>
+      <c r="BN161"/>
+      <c r="BO161"/>
+      <c r="BP161"/>
+      <c r="BQ161"/>
+      <c r="BR161"/>
+      <c r="BS161"/>
+      <c r="BT161"/>
+      <c r="BU161"/>
+      <c r="BV161"/>
+      <c r="BW161"/>
+      <c r="BX161"/>
+      <c r="BY161"/>
+      <c r="BZ161"/>
+      <c r="CA161"/>
+      <c r="CB161"/>
+      <c r="CC161"/>
+      <c r="CD161"/>
+      <c r="CE161"/>
+      <c r="CF161"/>
+      <c r="CG161"/>
+      <c r="CH161"/>
+      <c r="CI161"/>
+      <c r="CJ161"/>
+      <c r="CK161"/>
+      <c r="CL161"/>
+      <c r="CM161"/>
+      <c r="CN161"/>
+      <c r="CO161"/>
+      <c r="CP161"/>
+      <c r="CQ161"/>
+      <c r="CR161"/>
+      <c r="CS161"/>
+      <c r="CT161"/>
+      <c r="CU161"/>
+      <c r="CV161"/>
+      <c r="CW161"/>
+      <c r="CX161"/>
+      <c r="CY161"/>
+      <c r="CZ161"/>
+      <c r="DA161"/>
+      <c r="DB161"/>
+      <c r="DC161"/>
+      <c r="DD161"/>
+      <c r="DE161"/>
+      <c r="DF161"/>
+      <c r="DG161"/>
+      <c r="DH161"/>
+      <c r="DI161"/>
+      <c r="DJ161"/>
+      <c r="DK161"/>
+      <c r="DL161"/>
+      <c r="DM161"/>
+      <c r="DN161"/>
+      <c r="DO161"/>
+      <c r="DP161"/>
+      <c r="DQ161"/>
+      <c r="DR161"/>
+    </row>
+    <row r="162" spans="1:122" x14ac:dyDescent="0.35">
+      <c r="A162" s="61" t="s">
         <v>109</v>
       </c>
-      <c r="B155" s="2"/>
-      <c r="C155" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D155" s="69">
+      <c r="B162" s="2"/>
+      <c r="C162" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D162" s="69">
         <v>46230</v>
       </c>
-      <c r="E155" s="72"/>
-    </row>
-    <row r="156" spans="1:122" x14ac:dyDescent="0.35">
-      <c r="A156" s="60" t="s">
+      <c r="E162" s="72"/>
+    </row>
+    <row r="163" spans="1:122" x14ac:dyDescent="0.35">
+      <c r="A163" s="60" t="s">
         <v>26</v>
-      </c>
-      <c r="B156" s="2"/>
-      <c r="C156" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D156" s="69">
-        <v>46245</v>
-      </c>
-      <c r="E156" s="72"/>
-    </row>
-    <row r="157" spans="1:122" x14ac:dyDescent="0.35">
-      <c r="A157" s="61" t="s">
-        <v>17</v>
-      </c>
-      <c r="B157" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="C157" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D157" s="69">
-        <v>46260</v>
-      </c>
-      <c r="E157" s="72"/>
-    </row>
-    <row r="158" spans="1:122" x14ac:dyDescent="0.35">
-      <c r="A158" s="61" t="s">
-        <v>25</v>
-      </c>
-      <c r="B158" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C158" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D158" s="69">
-        <v>46282</v>
-      </c>
-      <c r="E158" s="72" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="159" spans="1:122" x14ac:dyDescent="0.35">
-      <c r="A159" s="61" t="s">
-        <v>108</v>
-      </c>
-      <c r="B159" s="2"/>
-      <c r="C159" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D159" s="69">
-        <v>46307</v>
-      </c>
-      <c r="E159" s="72"/>
-    </row>
-    <row r="160" spans="1:122" x14ac:dyDescent="0.35">
-      <c r="A160" s="61" t="s">
-        <v>89</v>
-      </c>
-      <c r="B160" s="2"/>
-      <c r="C160" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D160" s="69">
-        <v>46313</v>
-      </c>
-      <c r="E160" s="72"/>
-    </row>
-    <row r="161" spans="1:122" x14ac:dyDescent="0.35">
-      <c r="A161" s="60" t="s">
-        <v>34</v>
-      </c>
-      <c r="B161" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="C161" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D161" s="69">
-        <v>46319</v>
-      </c>
-      <c r="E161" s="72"/>
-    </row>
-    <row r="162" spans="1:122" x14ac:dyDescent="0.35">
-      <c r="A162" s="60" t="s">
-        <v>7</v>
-      </c>
-      <c r="B162" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C162" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D162" s="69">
-        <v>46320</v>
-      </c>
-      <c r="E162" s="72"/>
-    </row>
-    <row r="163" spans="1:122" x14ac:dyDescent="0.35">
-      <c r="A163" s="61" t="s">
-        <v>107</v>
       </c>
       <c r="B163" s="2"/>
       <c r="C163" s="2" t="s">
         <v>27</v>
       </c>
       <c r="D163" s="69">
-        <v>46328</v>
+        <v>46245</v>
       </c>
       <c r="E163" s="72"/>
     </row>
     <row r="164" spans="1:122" x14ac:dyDescent="0.35">
       <c r="A164" s="61" t="s">
-        <v>194</v>
+        <v>17</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>19</v>
+        <v>214</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>187</v>
+        <v>14</v>
       </c>
       <c r="D164" s="69">
-        <v>46329</v>
+        <v>46260</v>
       </c>
       <c r="E164" s="72"/>
     </row>
     <row r="165" spans="1:122" x14ac:dyDescent="0.35">
-      <c r="A165" s="60" t="s">
-        <v>18</v>
-      </c>
-      <c r="B165" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="C165" s="2" t="s">
+      <c r="A165" s="124" t="s">
+        <v>25</v>
+      </c>
+      <c r="B165" s="50" t="s">
+        <v>97</v>
+      </c>
+      <c r="C165" s="50" t="s">
+        <v>111</v>
+      </c>
+      <c r="D165" s="140">
+        <v>46282</v>
+      </c>
+      <c r="E165" s="72" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="166" spans="1:122" x14ac:dyDescent="0.35">
+      <c r="A166" s="61" t="s">
+        <v>108</v>
+      </c>
+      <c r="B166" s="2"/>
+      <c r="C166" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D166" s="69">
+        <v>46307</v>
+      </c>
+      <c r="E166" s="72"/>
+    </row>
+    <row r="167" spans="1:122" x14ac:dyDescent="0.35">
+      <c r="A167" s="61" t="s">
+        <v>89</v>
+      </c>
+      <c r="B167" s="2"/>
+      <c r="C167" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D167" s="69">
+        <v>46313</v>
+      </c>
+      <c r="E167" s="72"/>
+    </row>
+    <row r="168" spans="1:122" x14ac:dyDescent="0.35">
+      <c r="A168" s="60" t="s">
+        <v>34</v>
+      </c>
+      <c r="B168" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="C168" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D165" s="69">
-        <v>46358</v>
-      </c>
-      <c r="E165" s="72"/>
-    </row>
-    <row r="166" spans="1:122" x14ac:dyDescent="0.35">
-      <c r="A166" s="60" t="s">
-        <v>54</v>
-      </c>
-      <c r="B166" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C166" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D166" s="69">
-        <v>46387</v>
-      </c>
-      <c r="E166" s="72"/>
-    </row>
-    <row r="167" spans="1:122" x14ac:dyDescent="0.35">
-      <c r="A167" s="60" t="s">
-        <v>59</v>
-      </c>
-      <c r="B167" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C167" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D167" s="69">
-        <v>46387</v>
-      </c>
-      <c r="E167" s="72"/>
-    </row>
-    <row r="168" spans="1:122" x14ac:dyDescent="0.35">
-      <c r="A168" s="137" t="s">
-        <v>39</v>
-      </c>
-      <c r="B168" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C168" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="D168" s="69">
-        <v>46387</v>
+        <v>46319</v>
       </c>
       <c r="E168" s="72"/>
     </row>
     <row r="169" spans="1:122" x14ac:dyDescent="0.35">
       <c r="A169" s="60" t="s">
-        <v>56</v>
+        <v>7</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>27</v>
+        <v>99</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>27</v>
+        <v>100</v>
       </c>
       <c r="D169" s="69">
-        <v>46387</v>
+        <v>46320</v>
       </c>
       <c r="E169" s="72"/>
     </row>
     <row r="170" spans="1:122" x14ac:dyDescent="0.35">
-      <c r="A170" s="60" t="s">
-        <v>50</v>
-      </c>
-      <c r="B170" s="2" t="s">
-        <v>27</v>
-      </c>
+      <c r="A170" s="61" t="s">
+        <v>107</v>
+      </c>
+      <c r="B170" s="2"/>
       <c r="C170" s="2" t="s">
         <v>27</v>
       </c>
       <c r="D170" s="69">
-        <v>46387</v>
+        <v>46328</v>
       </c>
       <c r="E170" s="72"/>
     </row>
-    <row r="171" spans="1:122" s="55" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A171" s="60" t="s">
-        <v>3</v>
+    <row r="171" spans="1:122" x14ac:dyDescent="0.35">
+      <c r="A171" s="61" t="s">
+        <v>194</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>128</v>
+        <v>19</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>14</v>
+        <v>187</v>
       </c>
       <c r="D171" s="69">
-        <v>46387</v>
+        <v>46329</v>
       </c>
       <c r="E171" s="72"/>
-      <c r="F171"/>
-      <c r="G171"/>
-      <c r="H171"/>
-      <c r="I171"/>
-      <c r="J171"/>
-      <c r="K171"/>
-      <c r="L171"/>
-      <c r="M171"/>
-      <c r="N171"/>
-      <c r="O171"/>
-      <c r="P171"/>
-      <c r="Q171"/>
-      <c r="R171"/>
-      <c r="S171"/>
-      <c r="T171"/>
-      <c r="U171"/>
-      <c r="V171"/>
-      <c r="W171"/>
-      <c r="X171"/>
-      <c r="Y171"/>
-      <c r="Z171"/>
-      <c r="AA171"/>
-      <c r="AB171"/>
-      <c r="AC171"/>
-      <c r="AD171"/>
-      <c r="AE171"/>
-      <c r="AF171"/>
-      <c r="AG171"/>
-      <c r="AH171"/>
-      <c r="AI171"/>
-      <c r="AJ171"/>
-      <c r="AK171"/>
-      <c r="AL171"/>
-      <c r="AM171"/>
-      <c r="AN171"/>
-      <c r="AO171"/>
-      <c r="AP171"/>
-      <c r="AQ171"/>
-      <c r="AR171"/>
-      <c r="AS171"/>
-      <c r="AT171"/>
-      <c r="AU171"/>
-      <c r="AV171"/>
-      <c r="AW171"/>
-      <c r="AX171"/>
-      <c r="AY171"/>
-      <c r="AZ171"/>
-      <c r="BA171"/>
-      <c r="BB171"/>
-      <c r="BC171"/>
-      <c r="BD171"/>
-      <c r="BE171"/>
-      <c r="BF171"/>
-      <c r="BG171"/>
-      <c r="BH171"/>
-      <c r="BI171"/>
-      <c r="BJ171"/>
-      <c r="BK171"/>
-      <c r="BL171"/>
-      <c r="BM171"/>
-      <c r="BN171"/>
-      <c r="BO171"/>
-      <c r="BP171"/>
-      <c r="BQ171"/>
-      <c r="BR171"/>
-      <c r="BS171"/>
-      <c r="BT171"/>
-      <c r="BU171"/>
-      <c r="BV171"/>
-      <c r="BW171"/>
-      <c r="BX171"/>
-      <c r="BY171"/>
-      <c r="BZ171"/>
-      <c r="CA171"/>
-      <c r="CB171"/>
-      <c r="CC171"/>
-      <c r="CD171"/>
-      <c r="CE171"/>
-      <c r="CF171"/>
-      <c r="CG171"/>
-      <c r="CH171"/>
-      <c r="CI171"/>
-      <c r="CJ171"/>
-      <c r="CK171"/>
-      <c r="CL171"/>
-      <c r="CM171"/>
-      <c r="CN171"/>
-      <c r="CO171"/>
-      <c r="CP171"/>
-      <c r="CQ171"/>
-      <c r="CR171"/>
-      <c r="CS171"/>
-      <c r="CT171"/>
-      <c r="CU171"/>
-      <c r="CV171"/>
-      <c r="CW171"/>
-      <c r="CX171"/>
-      <c r="CY171"/>
-      <c r="CZ171"/>
-      <c r="DA171"/>
-      <c r="DB171"/>
-      <c r="DC171"/>
-      <c r="DD171"/>
-      <c r="DE171"/>
-      <c r="DF171"/>
-      <c r="DG171"/>
-      <c r="DH171"/>
-      <c r="DI171"/>
-      <c r="DJ171"/>
-      <c r="DK171"/>
-      <c r="DL171"/>
-      <c r="DM171"/>
-      <c r="DN171"/>
-      <c r="DO171"/>
-      <c r="DP171"/>
-      <c r="DQ171"/>
-      <c r="DR171"/>
     </row>
     <row r="172" spans="1:122" x14ac:dyDescent="0.35">
-      <c r="A172" s="61" t="s">
-        <v>17</v>
+      <c r="A172" s="60" t="s">
+        <v>18</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>83</v>
+        <v>174</v>
       </c>
       <c r="C172" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D172" s="69">
-        <v>46389</v>
+        <v>46358</v>
       </c>
       <c r="E172" s="72"/>
     </row>
     <row r="173" spans="1:122" x14ac:dyDescent="0.35">
-      <c r="A173" s="60" t="s">
-        <v>192</v>
+      <c r="A173" s="61" t="s">
+        <v>252</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>27</v>
+        <v>100</v>
       </c>
       <c r="D173" s="69">
-        <v>46487</v>
+        <v>46387</v>
       </c>
       <c r="E173" s="72"/>
     </row>
     <row r="174" spans="1:122" x14ac:dyDescent="0.35">
       <c r="A174" s="60" t="s">
+        <v>54</v>
+      </c>
+      <c r="B174" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C174" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D174" s="69">
+        <v>46387</v>
+      </c>
+      <c r="E174" s="72"/>
+    </row>
+    <row r="175" spans="1:122" x14ac:dyDescent="0.35">
+      <c r="A175" s="60" t="s">
+        <v>59</v>
+      </c>
+      <c r="B175" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C175" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D175" s="69">
+        <v>46387</v>
+      </c>
+      <c r="E175" s="72"/>
+    </row>
+    <row r="176" spans="1:122" x14ac:dyDescent="0.35">
+      <c r="A176" s="134" t="s">
+        <v>39</v>
+      </c>
+      <c r="B176" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C176" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D176" s="69">
+        <v>46387</v>
+      </c>
+      <c r="E176" s="72"/>
+    </row>
+    <row r="177" spans="1:122" x14ac:dyDescent="0.35">
+      <c r="A177" s="60" t="s">
+        <v>56</v>
+      </c>
+      <c r="B177" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C177" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D177" s="69">
+        <v>46387</v>
+      </c>
+      <c r="E177" s="72"/>
+    </row>
+    <row r="178" spans="1:122" x14ac:dyDescent="0.35">
+      <c r="A178" s="60" t="s">
+        <v>50</v>
+      </c>
+      <c r="B178" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C178" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D178" s="69">
+        <v>46387</v>
+      </c>
+      <c r="E178" s="72"/>
+    </row>
+    <row r="179" spans="1:122" s="55" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A179" s="60" t="s">
+        <v>3</v>
+      </c>
+      <c r="B179" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C179" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D179" s="69">
+        <v>46387</v>
+      </c>
+      <c r="E179" s="72"/>
+      <c r="F179"/>
+      <c r="G179"/>
+      <c r="H179"/>
+      <c r="I179"/>
+      <c r="J179"/>
+      <c r="K179"/>
+      <c r="L179"/>
+      <c r="M179"/>
+      <c r="N179"/>
+      <c r="O179"/>
+      <c r="P179"/>
+      <c r="Q179"/>
+      <c r="R179"/>
+      <c r="S179"/>
+      <c r="T179"/>
+      <c r="U179"/>
+      <c r="V179"/>
+      <c r="W179"/>
+      <c r="X179"/>
+      <c r="Y179"/>
+      <c r="Z179"/>
+      <c r="AA179"/>
+      <c r="AB179"/>
+      <c r="AC179"/>
+      <c r="AD179"/>
+      <c r="AE179"/>
+      <c r="AF179"/>
+      <c r="AG179"/>
+      <c r="AH179"/>
+      <c r="AI179"/>
+      <c r="AJ179"/>
+      <c r="AK179"/>
+      <c r="AL179"/>
+      <c r="AM179"/>
+      <c r="AN179"/>
+      <c r="AO179"/>
+      <c r="AP179"/>
+      <c r="AQ179"/>
+      <c r="AR179"/>
+      <c r="AS179"/>
+      <c r="AT179"/>
+      <c r="AU179"/>
+      <c r="AV179"/>
+      <c r="AW179"/>
+      <c r="AX179"/>
+      <c r="AY179"/>
+      <c r="AZ179"/>
+      <c r="BA179"/>
+      <c r="BB179"/>
+      <c r="BC179"/>
+      <c r="BD179"/>
+      <c r="BE179"/>
+      <c r="BF179"/>
+      <c r="BG179"/>
+      <c r="BH179"/>
+      <c r="BI179"/>
+      <c r="BJ179"/>
+      <c r="BK179"/>
+      <c r="BL179"/>
+      <c r="BM179"/>
+      <c r="BN179"/>
+      <c r="BO179"/>
+      <c r="BP179"/>
+      <c r="BQ179"/>
+      <c r="BR179"/>
+      <c r="BS179"/>
+      <c r="BT179"/>
+      <c r="BU179"/>
+      <c r="BV179"/>
+      <c r="BW179"/>
+      <c r="BX179"/>
+      <c r="BY179"/>
+      <c r="BZ179"/>
+      <c r="CA179"/>
+      <c r="CB179"/>
+      <c r="CC179"/>
+      <c r="CD179"/>
+      <c r="CE179"/>
+      <c r="CF179"/>
+      <c r="CG179"/>
+      <c r="CH179"/>
+      <c r="CI179"/>
+      <c r="CJ179"/>
+      <c r="CK179"/>
+      <c r="CL179"/>
+      <c r="CM179"/>
+      <c r="CN179"/>
+      <c r="CO179"/>
+      <c r="CP179"/>
+      <c r="CQ179"/>
+      <c r="CR179"/>
+      <c r="CS179"/>
+      <c r="CT179"/>
+      <c r="CU179"/>
+      <c r="CV179"/>
+      <c r="CW179"/>
+      <c r="CX179"/>
+      <c r="CY179"/>
+      <c r="CZ179"/>
+      <c r="DA179"/>
+      <c r="DB179"/>
+      <c r="DC179"/>
+      <c r="DD179"/>
+      <c r="DE179"/>
+      <c r="DF179"/>
+      <c r="DG179"/>
+      <c r="DH179"/>
+      <c r="DI179"/>
+      <c r="DJ179"/>
+      <c r="DK179"/>
+      <c r="DL179"/>
+      <c r="DM179"/>
+      <c r="DN179"/>
+      <c r="DO179"/>
+      <c r="DP179"/>
+      <c r="DQ179"/>
+      <c r="DR179"/>
+    </row>
+    <row r="180" spans="1:122" x14ac:dyDescent="0.35">
+      <c r="A180" s="61" t="s">
+        <v>17</v>
+      </c>
+      <c r="B180" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C180" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D180" s="69">
+        <v>46389</v>
+      </c>
+      <c r="E180" s="72"/>
+    </row>
+    <row r="181" spans="1:122" x14ac:dyDescent="0.35">
+      <c r="A181" s="60" t="s">
+        <v>65</v>
+      </c>
+      <c r="B181" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C181" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D181" s="69">
+        <v>46477</v>
+      </c>
+      <c r="E181" s="72"/>
+    </row>
+    <row r="182" spans="1:122" x14ac:dyDescent="0.35">
+      <c r="A182" s="60" t="s">
+        <v>192</v>
+      </c>
+      <c r="B182" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C182" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D182" s="69">
+        <v>46487</v>
+      </c>
+      <c r="E182" s="72"/>
+    </row>
+    <row r="183" spans="1:122" x14ac:dyDescent="0.35">
+      <c r="A183" s="60" t="s">
         <v>63</v>
       </c>
-      <c r="B174" s="2" t="s">
+      <c r="B183" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="C174" s="2" t="s">
+      <c r="C183" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D174" s="69">
+      <c r="D183" s="69">
         <v>47029</v>
       </c>
-      <c r="E174" s="72"/>
-    </row>
-    <row r="175" spans="1:122" x14ac:dyDescent="0.35">
-      <c r="A175" s="60"/>
-      <c r="B175" s="2"/>
-      <c r="C175" s="2"/>
-      <c r="D175" s="69"/>
-      <c r="E175" s="72"/>
-    </row>
-    <row r="176" spans="1:122" x14ac:dyDescent="0.35">
-      <c r="A176" s="60"/>
-      <c r="B176" s="2"/>
-      <c r="C176" s="2"/>
-      <c r="D176" s="69"/>
-      <c r="E176" s="72"/>
-    </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A177" s="61"/>
-      <c r="B177" s="2"/>
-      <c r="C177" s="2"/>
-      <c r="D177" s="69"/>
-      <c r="E177" s="72"/>
-    </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A178" s="60"/>
-      <c r="B178" s="2"/>
-      <c r="C178" s="2"/>
-      <c r="D178" s="69"/>
-      <c r="E178" s="72"/>
+      <c r="E183" s="72"/>
+    </row>
+    <row r="184" spans="1:122" x14ac:dyDescent="0.35">
+      <c r="A184" s="60"/>
+      <c r="B184" s="2"/>
+      <c r="C184" s="2"/>
+      <c r="D184" s="69"/>
+      <c r="E184" s="72"/>
+    </row>
+    <row r="185" spans="1:122" x14ac:dyDescent="0.35">
+      <c r="A185" s="60"/>
+      <c r="B185" s="2"/>
+      <c r="C185" s="2"/>
+      <c r="D185" s="69"/>
+      <c r="E185" s="72"/>
+    </row>
+    <row r="186" spans="1:122" x14ac:dyDescent="0.35">
+      <c r="A186" s="61"/>
+      <c r="B186" s="2"/>
+      <c r="C186" s="2"/>
+      <c r="D186" s="69"/>
+      <c r="E186" s="72"/>
+    </row>
+    <row r="187" spans="1:122" x14ac:dyDescent="0.35">
+      <c r="A187" s="60"/>
+      <c r="B187" s="2"/>
+      <c r="C187" s="2"/>
+      <c r="D187" s="69"/>
+      <c r="E187" s="72"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -4995,13 +5384,13 @@
     <hyperlink ref="A86" r:id="rId27" xr:uid="{EF9E5405-0057-4913-BB66-8DADEA3ADAC1}"/>
     <hyperlink ref="A87" r:id="rId28" xr:uid="{77AD3351-401A-45BD-B406-81289E91E2B7}"/>
     <hyperlink ref="A93" r:id="rId29" xr:uid="{7488D608-8004-4897-996F-BC8BACB78819}"/>
-    <hyperlink ref="A151" r:id="rId30" xr:uid="{216B7BB1-9833-42F6-8BD6-FCD583005659}"/>
-    <hyperlink ref="A154" r:id="rId31" xr:uid="{FA25EFB8-9CF4-4906-BA52-DDB4946ED57F}"/>
-    <hyperlink ref="A171" r:id="rId32" xr:uid="{6DC17469-2AE4-486A-B2FB-692C612C938F}"/>
+    <hyperlink ref="A156" r:id="rId30" xr:uid="{216B7BB1-9833-42F6-8BD6-FCD583005659}"/>
+    <hyperlink ref="A161" r:id="rId31" xr:uid="{FA25EFB8-9CF4-4906-BA52-DDB4946ED57F}"/>
+    <hyperlink ref="A179" r:id="rId32" xr:uid="{6DC17469-2AE4-486A-B2FB-692C612C938F}"/>
     <hyperlink ref="A19" r:id="rId33" xr:uid="{0D893380-8851-499C-B099-36DE61DF32F5}"/>
     <hyperlink ref="A21" r:id="rId34" xr:uid="{87B26A19-7710-44FB-B821-04076D6AFBF0}"/>
     <hyperlink ref="A35" r:id="rId35" xr:uid="{E391FA3E-2D35-4729-830F-6D61CBEC0188}"/>
-    <hyperlink ref="A162" r:id="rId36" xr:uid="{2CACF691-BB8F-4886-AC93-9CE1A774C547}"/>
+    <hyperlink ref="A169" r:id="rId36" xr:uid="{2CACF691-BB8F-4886-AC93-9CE1A774C547}"/>
     <hyperlink ref="A13" r:id="rId37" xr:uid="{C4EC3C20-6E17-4496-AE8C-0CEF0E9A227E}"/>
     <hyperlink ref="A18" r:id="rId38" xr:uid="{DE7A9130-E078-4D30-B625-191B5DB108EB}"/>
     <hyperlink ref="A15" r:id="rId39" xr:uid="{BE9D8063-99E0-4594-B7AE-033FE54B7D57}"/>
@@ -5010,7 +5399,7 @@
     <hyperlink ref="A49" r:id="rId42" xr:uid="{AA26D797-BF58-4D70-80DD-349BD90AC78D}"/>
     <hyperlink ref="A47" r:id="rId43" display="http://10.0.10.4/link/A4CAE6F5-E38B-46FC-8A73-E356A04AAB61/show?object=2BAC4AEF-5562-4507-9D44-9918AC72C412&amp;objid=0-34910" xr:uid="{E1078946-D888-434A-9235-9A9ADAE1F358}"/>
     <hyperlink ref="A31" r:id="rId44" xr:uid="{13658346-E407-4C32-B12D-1EE442E6D4C1}"/>
-    <hyperlink ref="A165" r:id="rId45" xr:uid="{F8667B27-785F-4C86-8CBE-F02D36031873}"/>
+    <hyperlink ref="A172" r:id="rId45" xr:uid="{F8667B27-785F-4C86-8CBE-F02D36031873}"/>
     <hyperlink ref="A38" r:id="rId46" xr:uid="{3384F468-C50F-4198-92F5-4021B95195D6}"/>
     <hyperlink ref="A30" r:id="rId47" xr:uid="{F5DBA126-4925-4CE7-BF0A-F16F60CFE40E}"/>
     <hyperlink ref="A41" r:id="rId48" xr:uid="{4270CE8F-9570-4350-950E-4CDF1AF1DAE7}"/>
@@ -5020,7 +5409,7 @@
     <hyperlink ref="A112" r:id="rId52" xr:uid="{F9CF7289-D6A0-4780-87E7-3B78286AB288}"/>
     <hyperlink ref="A128" r:id="rId53" display="http://10.0.10.4/link/A4CAE6F5-E38B-46FC-8A73-E356A04AAB61/show?object=2BAC4AEF-5562-4507-9D44-9918AC72C412&amp;objid=0-34910" xr:uid="{9CFE415C-C17B-490C-8037-2532E86DE931}"/>
     <hyperlink ref="A55" r:id="rId54" xr:uid="{F9D9DEAA-53C8-468C-8630-D40E5EFE2D71}"/>
-    <hyperlink ref="A138" r:id="rId55" xr:uid="{78BB742D-73FF-403F-AD77-3A21BEA8FABD}"/>
+    <hyperlink ref="A142" r:id="rId55" xr:uid="{78BB742D-73FF-403F-AD77-3A21BEA8FABD}"/>
     <hyperlink ref="A115" r:id="rId56" xr:uid="{D4C47D54-2008-4878-8D6C-0A5103A83E1C}"/>
     <hyperlink ref="A36" r:id="rId57" xr:uid="{5C9626EA-E4A5-4D0E-B953-6B4B82F709E2}"/>
     <hyperlink ref="A37" r:id="rId58" xr:uid="{96654049-8A20-4712-8E12-BB280F6D48FA}"/>
@@ -5031,7 +5420,7 @@
     <hyperlink ref="A69" r:id="rId63" xr:uid="{36B5D324-9B53-4B8D-903E-0AFF9FF40F68}"/>
     <hyperlink ref="A54" r:id="rId64" xr:uid="{B0D7BE6C-2A85-487A-8233-DA7B4990ADD3}"/>
     <hyperlink ref="A64" r:id="rId65" xr:uid="{DC598FAA-2E8D-49B9-8196-77EFABE48390}"/>
-    <hyperlink ref="A173" r:id="rId66" xr:uid="{2A55D894-3782-4A93-BFF5-8BB45EF3BC96}"/>
+    <hyperlink ref="A182" r:id="rId66" xr:uid="{2A55D894-3782-4A93-BFF5-8BB45EF3BC96}"/>
     <hyperlink ref="A124" r:id="rId67" xr:uid="{703A2AC6-9444-4E57-ABFB-EE6ED7C9D085}"/>
     <hyperlink ref="A60" r:id="rId68" xr:uid="{542D71B6-F1E7-4AE6-B1FA-65A7E15CE5C1}"/>
     <hyperlink ref="A78" r:id="rId69" xr:uid="{F4B4F6EC-E5D9-4E63-B04A-BEB38A3599C0}"/>
@@ -5046,27 +5435,34 @@
     <hyperlink ref="A73" r:id="rId78" xr:uid="{53E5BB95-7747-494E-8B3F-CE8985BCCD8C}"/>
     <hyperlink ref="A77" r:id="rId79" xr:uid="{BD73F50C-8C2C-4097-AC56-2AC6085BA386}"/>
     <hyperlink ref="A81" r:id="rId80" xr:uid="{D8195D1C-89BE-48B0-ACCE-AC0D6F84221D}"/>
-    <hyperlink ref="A156" r:id="rId81" xr:uid="{3FADFDCB-7E5E-4791-B644-7806EF4F9053}"/>
+    <hyperlink ref="A163" r:id="rId81" xr:uid="{3FADFDCB-7E5E-4791-B644-7806EF4F9053}"/>
     <hyperlink ref="A95" r:id="rId82" xr:uid="{763050C7-E204-49E6-8F57-0D2A8A2AFEC5}"/>
     <hyperlink ref="A99" r:id="rId83" xr:uid="{A872B1D5-9CB2-4BF6-B70C-E785B0081A1C}"/>
     <hyperlink ref="A100" r:id="rId84" xr:uid="{13305418-280C-4A0F-8F52-F89EB87E7464}"/>
-    <hyperlink ref="A145" r:id="rId85" xr:uid="{02545752-74FC-4347-ABE9-9F3945601C86}"/>
+    <hyperlink ref="A150" r:id="rId85" xr:uid="{02545752-74FC-4347-ABE9-9F3945601C86}"/>
     <hyperlink ref="A127" r:id="rId86" xr:uid="{2BAC6AD7-0236-4814-99E0-82B25FD9E481}"/>
     <hyperlink ref="A122" r:id="rId87" xr:uid="{CF52E32D-755C-49FF-80CB-BB902CF11B42}"/>
-    <hyperlink ref="A161" r:id="rId88" xr:uid="{2A771FF4-F864-4AE6-9A3E-0D5C86951B7A}"/>
-    <hyperlink ref="A174" r:id="rId89" xr:uid="{2B519212-7208-4B3F-8C3B-6CB1677D1E24}"/>
+    <hyperlink ref="A168" r:id="rId88" xr:uid="{2A771FF4-F864-4AE6-9A3E-0D5C86951B7A}"/>
+    <hyperlink ref="A183" r:id="rId89" xr:uid="{2B519212-7208-4B3F-8C3B-6CB1677D1E24}"/>
     <hyperlink ref="A121" r:id="rId90" xr:uid="{86BB471B-F7BD-4FC7-B274-E6257B5430F7}"/>
     <hyperlink ref="A97" r:id="rId91" xr:uid="{7A586C77-7A05-4E91-83B8-6B5C0FD22752}"/>
-    <hyperlink ref="A170" r:id="rId92" xr:uid="{5B632E0F-4D33-40DC-8C56-9D8A3A64DDF4}"/>
-    <hyperlink ref="A167" r:id="rId93" xr:uid="{F9707FAA-2528-441B-A8E3-90694B09A0F9}"/>
-    <hyperlink ref="A169" r:id="rId94" xr:uid="{79837541-2DC6-4F63-AA38-276A6FC31426}"/>
-    <hyperlink ref="A153" r:id="rId95" xr:uid="{4B736B0C-7002-4E53-9963-F457726B67A4}"/>
-    <hyperlink ref="A152" r:id="rId96" xr:uid="{9FAC6E36-AE7B-4D72-9D2A-E6B4BAC03F19}"/>
+    <hyperlink ref="A178" r:id="rId92" xr:uid="{5B632E0F-4D33-40DC-8C56-9D8A3A64DDF4}"/>
+    <hyperlink ref="A175" r:id="rId93" xr:uid="{F9707FAA-2528-441B-A8E3-90694B09A0F9}"/>
+    <hyperlink ref="A177" r:id="rId94" xr:uid="{79837541-2DC6-4F63-AA38-276A6FC31426}"/>
+    <hyperlink ref="A159" r:id="rId95" xr:uid="{4B736B0C-7002-4E53-9963-F457726B67A4}"/>
+    <hyperlink ref="A158" r:id="rId96" xr:uid="{9FAC6E36-AE7B-4D72-9D2A-E6B4BAC03F19}"/>
     <hyperlink ref="A131" r:id="rId97" xr:uid="{4E3A922C-5FA1-437C-A138-E27A0AB81A85}"/>
-    <hyperlink ref="A137" r:id="rId98" xr:uid="{24D5EE0D-E898-40D1-BACB-35BC01593C2A}"/>
+    <hyperlink ref="A140" r:id="rId98" xr:uid="{24D5EE0D-E898-40D1-BACB-35BC01593C2A}"/>
+    <hyperlink ref="A147" r:id="rId99" xr:uid="{5D4C087D-6199-48E3-B933-FA81772E4EA0}"/>
+    <hyperlink ref="A181" r:id="rId100" xr:uid="{74C92563-22E4-4585-82BB-A4ACBA191AF2}"/>
+    <hyperlink ref="A157" r:id="rId101" xr:uid="{142C2334-40BB-4EED-8EFB-849EC5A71EBA}"/>
+    <hyperlink ref="A160" r:id="rId102" xr:uid="{3D499344-5F60-42EA-B73C-EA71BC7797E3}"/>
+    <hyperlink ref="A138" r:id="rId103" xr:uid="{4A942445-8164-4D10-AD50-A2BFCB3725D6}"/>
+    <hyperlink ref="A137" r:id="rId104" xr:uid="{9E3E3393-2CDD-49D9-B3C7-01CBDDF04149}"/>
+    <hyperlink ref="A139" r:id="rId105" xr:uid="{F53F5054-6B7D-4981-B0E6-406539CB1C88}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="8" scale="70" orientation="landscape" r:id="rId99"/>
+  <pageSetup paperSize="8" scale="70" orientation="landscape" r:id="rId106"/>
 </worksheet>
 </file>
 

</xml_diff>